<commit_message>
exclude more columns, fixed a bug with search_author
</commit_message>
<xml_diff>
--- a/DOM_Banner/output/dept0721/HH Sherry Chow_2023.xlsx
+++ b/DOM_Banner/output/dept0721/HH Sherry Chow_2023.xlsx
@@ -1944,7 +1944,7 @@
       </c>
       <c r="AF9" t="inlineStr">
         <is>
-          <t>c("https://openalex.org/W2044330087", "https://openalex.org/W4361814968", "https://openalex.org/W4361814985", "https://openalex.org/W4361814998", "https://openalex.org/W4361814935", "https://openalex.org/W4361815613", "https://openalex.org/W4361815443", "https://openalex.org/W4361939778", "https://openalex.org/W4361815217", "https://openalex.org/W4361939742")</t>
+          <t>c("https://openalex.org/W2063752897", "https://openalex.org/W2004287019", "https://openalex.org/W2385053099", "https://openalex.org/W2041850705", "https://openalex.org/W2409486576", "https://openalex.org/W1972333242", "https://openalex.org/W1968946548", "https://openalex.org/W2092792292", "https://openalex.org/W2110109601", "https://openalex.org/W1975307184")</t>
         </is>
       </c>
       <c r="AG9" t="inlineStr">
@@ -2469,7 +2469,7 @@
       </c>
       <c r="AF12" t="inlineStr">
         <is>
-          <t>c("https://openalex.org/W2131241813", "https://openalex.org/W2926335606", "https://openalex.org/W2110010322", "https://openalex.org/W2088005812", "https://openalex.org/W164398201", "https://openalex.org/W1964441320", "https://openalex.org/W2169905015", "https://openalex.org/W4237422067", "https://openalex.org/W2032603988", "https://openalex.org/W2012733509")</t>
+          <t>c("https://openalex.org/W2063752897", "https://openalex.org/W2004287019", "https://openalex.org/W2385053099", "https://openalex.org/W2041850705", "https://openalex.org/W2409486576", "https://openalex.org/W1972333242", "https://openalex.org/W1968946548", "https://openalex.org/W2092792292", "https://openalex.org/W2110109601", "https://openalex.org/W1975307184")</t>
         </is>
       </c>
       <c r="AG12" t="inlineStr">
@@ -3694,7 +3694,7 @@
       </c>
       <c r="AF19" t="inlineStr">
         <is>
-          <t>c("https://openalex.org/W4361814968", "https://openalex.org/W4361814985", "https://openalex.org/W4361814998", "https://openalex.org/W4361814935", "https://openalex.org/W4361815217", "https://openalex.org/W2044330087", "https://openalex.org/W4361815613", "https://openalex.org/W4361815443", "https://openalex.org/W4361939778", "https://openalex.org/W4361939742")</t>
+          <t>c("https://openalex.org/W2063752897", "https://openalex.org/W2004287019", "https://openalex.org/W2385053099", "https://openalex.org/W2041850705", "https://openalex.org/W2409486576", "https://openalex.org/W1972333242", "https://openalex.org/W1968946548", "https://openalex.org/W2092792292", "https://openalex.org/W2110109601", "https://openalex.org/W1975307184")</t>
         </is>
       </c>
       <c r="AG19" t="inlineStr">

</xml_diff>